<commit_message>
new plots and new r script
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carolyn/Desktop/Practice_Data_Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E494EE3-4CDA-A648-B006-E42BACFC8390}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE8F985F-7C8B-5F44-BAFB-A7A445730670}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test" sheetId="1" r:id="rId1"/>
@@ -921,7 +921,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1052,6 +1052,13 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1404,9 +1411,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1782,10 +1791,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:EO30"/>
+  <dimension ref="A1:EO36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CX1" workbookViewId="0">
-      <selection activeCell="DJ30" sqref="DJ30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2672,7 +2681,7 @@
       </c>
     </row>
     <row r="3" spans="1:145" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>147</v>
       </c>
       <c r="B3" t="s">
@@ -2687,7 +2696,7 @@
       <c r="E3">
         <v>0.206632656</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="2">
         <v>0.58273381300000004</v>
       </c>
       <c r="G3">
@@ -3109,7 +3118,7 @@
       </c>
     </row>
     <row r="4" spans="1:145" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>147</v>
       </c>
       <c r="B4" t="s">
@@ -3124,7 +3133,7 @@
       <c r="E4">
         <v>0.18347048799999999</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="2">
         <v>0.30215827299999998</v>
       </c>
       <c r="G4">
@@ -3546,7 +3555,7 @@
       </c>
     </row>
     <row r="5" spans="1:145" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>147</v>
       </c>
       <c r="B5" t="s">
@@ -3561,7 +3570,7 @@
       <c r="E5">
         <v>0.14272918800000001</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="2">
         <v>0.30215827299999998</v>
       </c>
       <c r="G5">
@@ -6168,7 +6177,7 @@
       </c>
     </row>
     <row r="11" spans="1:145" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="A11" s="2" t="s">
         <v>147</v>
       </c>
       <c r="B11" t="s">
@@ -6183,7 +6192,7 @@
       <c r="E11">
         <v>1.4209945E-2</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="2">
         <v>0.100719424</v>
       </c>
       <c r="G11">
@@ -6605,7 +6614,7 @@
       </c>
     </row>
     <row r="12" spans="1:145" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="A12" s="2" t="s">
         <v>147</v>
       </c>
       <c r="B12" t="s">
@@ -6620,7 +6629,7 @@
       <c r="E12">
         <v>1.4002356000000001E-2</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="2">
         <v>7.9136690999999995E-2</v>
       </c>
       <c r="G12">
@@ -7916,7 +7925,7 @@
       </c>
     </row>
     <row r="15" spans="1:145" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="A15" s="2" t="s">
         <v>147</v>
       </c>
       <c r="B15" t="s">
@@ -8790,7 +8799,7 @@
       </c>
     </row>
     <row r="17" spans="1:145" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="A17" s="2" t="s">
         <v>147</v>
       </c>
       <c r="B17" t="s">
@@ -8805,7 +8814,7 @@
       <c r="E17">
         <v>4.10371E-3</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="2">
         <v>7.1942450000000002E-3</v>
       </c>
       <c r="G17">
@@ -9227,7 +9236,7 @@
       </c>
     </row>
     <row r="18" spans="1:145" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="A18" s="2" t="s">
         <v>147</v>
       </c>
       <c r="B18" t="s">
@@ -9242,7 +9251,7 @@
       <c r="E18">
         <v>4.0944249999999996E-3</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="2">
         <v>0.12230215799999999</v>
       </c>
       <c r="G18">
@@ -9664,7 +9673,7 @@
       </c>
     </row>
     <row r="19" spans="1:145" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="A19" s="2" t="s">
         <v>147</v>
       </c>
       <c r="B19" t="s">
@@ -9679,7 +9688,7 @@
       <c r="E19">
         <v>3.9982569999999999E-3</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="2">
         <v>5.7553957000000003E-2</v>
       </c>
       <c r="G19">
@@ -10101,7 +10110,7 @@
       </c>
     </row>
     <row r="20" spans="1:145" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="A20" s="2" t="s">
         <v>147</v>
       </c>
       <c r="B20" t="s">
@@ -10116,7 +10125,7 @@
       <c r="E20">
         <v>3.7618170000000002E-3</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="2">
         <v>7.1942450000000002E-3</v>
       </c>
       <c r="G20">
@@ -10538,7 +10547,7 @@
       </c>
     </row>
     <row r="21" spans="1:145" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="A21" s="2" t="s">
         <v>147</v>
       </c>
       <c r="B21" t="s">
@@ -10553,7 +10562,7 @@
       <c r="E21">
         <v>3.4295409999999999E-3</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="2">
         <v>2.1582733999999999E-2</v>
       </c>
       <c r="G21">
@@ -12286,7 +12295,7 @@
       </c>
     </row>
     <row r="25" spans="1:145" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="A25" s="2" t="s">
         <v>147</v>
       </c>
       <c r="B25" t="s">
@@ -12301,7 +12310,7 @@
       <c r="E25">
         <v>2.4764850000000001E-3</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="2">
         <v>0.100719424</v>
       </c>
       <c r="G25">
@@ -14870,6 +14879,12 @@
       <c r="EO30" t="s">
         <v>293</v>
       </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E35" s="3"/>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B36" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>